<commit_message>
Added excel support for telegram.
</commit_message>
<xml_diff>
--- a/temp/IP-82/КПЗ.xlsx
+++ b/temp/IP-82/КПЗ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Студент</t>
   </si>
@@ -23,6 +23,9 @@
   </si>
   <si>
     <t>Бебех Олександр</t>
+  </si>
+  <si>
+    <t>Дзівідзінська Мар'яна</t>
   </si>
   <si>
     <t>Орлов Володимир</t>
@@ -386,7 +389,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -419,7 +422,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>70</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -430,6 +433,17 @@
         <v>4</v>
       </c>
       <c r="C4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
         <v>59</v>
       </c>
     </row>

</xml_diff>